<commit_message>
Pequenas modificacoes no codigo, e inclusao de comentarios
</commit_message>
<xml_diff>
--- a/dados_capturados/capturas.xlsx
+++ b/dados_capturados/capturas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,40 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-06-30 18:30:15</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16°C</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-06-30 18:30:47</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16°C</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>87%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusao de comentarios, e teste de captura.
</commit_message>
<xml_diff>
--- a/dados_capturados/capturas.xlsx
+++ b/dados_capturados/capturas.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,23 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-07-01 12:20:32</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>16°C</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>67%</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>